<commit_message>
Still getting column types working
</commit_message>
<xml_diff>
--- a/Tests/UnitTests/PreSimulationTools/Input.xlsx
+++ b/Tests/UnitTests/PreSimulationTools/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\UnitTests\PreSimulationTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4A2F6-5A5C-462C-A937-2E3B1412DC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E92F57-315B-42AD-BF88-DA141B8E083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{890001CA-2A37-4612-87E0-C6942AAFCBB2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>DayMonth</t>
   </si>
@@ -44,9 +44,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>1 Jan</t>
   </si>
   <si>
@@ -68,7 +65,19 @@
     <t>SimulationName</t>
   </si>
   <si>
-    <t>Simulation</t>
+    <t>Clock.Today</t>
+  </si>
+  <si>
+    <t>Wheat.Grain.Wt</t>
+  </si>
+  <si>
+    <t>ValueWithSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Wheat.Grain.N</t>
   </si>
 </sst>
 </file>
@@ -441,26 +450,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FA1752-1FF7-45FC-A016-CD46D3ACF35B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -468,47 +479,102 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding unit tests and icon
</commit_message>
<xml_diff>
--- a/Tests/UnitTests/PreSimulationTools/Input.xlsx
+++ b/Tests/UnitTests/PreSimulationTools/Input.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\UnitTests\PreSimulationTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E92F57-315B-42AD-BF88-DA141B8E083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310F10C0-9165-47B5-9182-6D2492FE1278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{890001CA-2A37-4612-87E0-C6942AAFCBB2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>DayMonth</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Wheat.Grain.N</t>
+  </si>
+  <si>
+    <t>Sim2</t>
+  </si>
+  <si>
+    <t>Sim3</t>
+  </si>
+  <si>
+    <t>Sim5</t>
+  </si>
+  <si>
+    <t>Simulation1</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FA1752-1FF7-45FC-A016-CD46D3ACF35B}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,8 +502,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -505,10 +517,13 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -530,8 +545,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -553,8 +568,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -567,14 +582,39 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
+      <c r="A6" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>